<commit_message>
Update table sp3, training set composition of other published ML algorithms
</commit_message>
<xml_diff>
--- a/Supplementary tables/Supplementary Table - Sp3.xlsx
+++ b/Supplementary tables/Supplementary Table - Sp3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Panda/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Panda/Documents/GitHub/baolab-rice/CRISPR_OT_scoring/Supplementary tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{666B542C-862F-7840-BFD6-2F312ED7EA4A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E2C6282-FE26-3B42-B2ED-51F842847D75}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24160" yWindow="9520" windowWidth="47640" windowHeight="26020" xr2:uid="{28E073DA-A9D1-AA45-B6B4-3D59C1EC5723}"/>
+    <workbookView xWindow="24160" yWindow="5920" windowWidth="47640" windowHeight="26020" xr2:uid="{28E073DA-A9D1-AA45-B6B4-3D59C1EC5723}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -195,7 +195,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -209,6 +209,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -530,7 +533,7 @@
   <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -555,13 +558,13 @@
       <c r="D1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B2" s="2"/>
@@ -583,89 +586,91 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="B3" s="4" t="s">
-        <v>11</v>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B3" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>30</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E3" s="2"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="G3" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="H3" s="2"/>
-      <c r="I3" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="F4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
+      <c r="I4" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>30</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E5" s="2"/>
       <c r="F5" s="2"/>
-      <c r="G5" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="G5" s="2"/>
       <c r="H5" s="2"/>
-      <c r="I5" s="1" t="s">
-        <v>30</v>
+      <c r="I5" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
+      <c r="F6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="I6" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>4</v>
@@ -674,87 +679,75 @@
         <v>5</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>3</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="F7" s="2"/>
       <c r="G7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="2"/>
+      <c r="I7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I7" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+    </row>
+    <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="6"/>
-      <c r="B9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="6"/>
-      <c r="B10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="G10" s="2"/>
       <c r="H10" s="2" t="s">
         <v>34</v>
       </c>
@@ -763,15 +756,15 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
+      <c r="A11" s="7"/>
       <c r="B11" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2" t="s">
@@ -786,21 +779,23 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="6"/>
+      <c r="A12" s="7"/>
       <c r="B12" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G12" s="2"/>
+      <c r="G12" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="H12" s="2" t="s">
         <v>34</v>
       </c>
@@ -809,12 +804,12 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="6"/>
+      <c r="A13" s="7"/>
       <c r="B13" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>7</v>
@@ -823,9 +818,7 @@
       <c r="F13" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="G13" s="2"/>
       <c r="H13" s="2" t="s">
         <v>34</v>
       </c>
@@ -834,15 +827,15 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="6"/>
+      <c r="A14" s="7"/>
       <c r="B14" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
@@ -857,11 +850,12 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="7"/>
       <c r="B15" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>7</v>
@@ -870,26 +864,35 @@
       <c r="F15" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
+      <c r="G15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="I15" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="7"/>
       <c r="B16" s="2" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
+      <c r="F16" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
+      <c r="H16" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="I16" s="2" t="s">
         <v>3</v>
       </c>
@@ -922,7 +925,7 @@
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="E1:I1"/>
-    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A10:A16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>